<commit_message>
fixed typo in peak map 18:2 9, 12
</commit_message>
<xml_diff>
--- a/data/IRMS/peak_map_manual.xlsx
+++ b/data/IRMS/peak_map_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/active_repos/tristan_d2o/data/IRMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\active_repos\tristan_d2o\data\IRMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9516198C-4941-1340-8AC9-9B74E917CC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B43BE5-3307-4B38-9169-DD5C79A336BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{42725BC7-9775-E54E-AA2D-819F4CD6C3D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{42725BC7-9775-E54E-AA2D-819F4CD6C3D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>17:0 cyclo</t>
   </si>
   <si>
-    <t>18:2 trans 9,12</t>
-  </si>
-  <si>
     <t>18:1 trans 9</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>rt:BF10900</t>
+  </si>
+  <si>
+    <t>18:2 trans 9, 12</t>
   </si>
 </sst>
 </file>
@@ -458,15 +458,15 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,13 +474,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -494,7 +494,7 @@
         <v>1702.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -508,7 +508,7 @@
         <v>1721.74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -522,7 +522,7 @@
         <v>1961.88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -536,7 +536,7 @@
         <v>2004.73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -550,7 +550,7 @@
         <v>2026.26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -564,7 +564,7 @@
         <v>2072.0300000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -578,7 +578,7 @@
         <v>2224.1799999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -592,9 +592,9 @@
         <v>2280.19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>2480.62</v>
@@ -606,9 +606,9 @@
         <v>2483.34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>2505.2800000000002</v>
@@ -620,9 +620,9 @@
         <v>2509.0500000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>2528.27</v>
@@ -634,9 +634,9 @@
         <v>2533.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2575.3000000000002</v>
@@ -648,9 +648,9 @@
         <v>2579.27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>2628.38</v>
@@ -662,9 +662,9 @@
         <v>2637.16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>3058.92</v>
@@ -676,9 +676,9 @@
         <v>3061.43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>3299.48</v>
@@ -690,9 +690,9 @@
         <v>3307.22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>3513.92</v>
@@ -704,9 +704,9 @@
         <v>3516.43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>3729.61</v>
@@ -718,9 +718,9 @@
         <v>3733.78</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>3794.81</v>
@@ -732,9 +732,9 @@
         <v>3796.28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>3936.72</v>

</xml_diff>